<commit_message>
Agregando federacion, persona y puesto
</commit_message>
<xml_diff>
--- a/docs/NUMEROS DE ASIGNACION DE EXPEDIENTES TEDEFE.xlsx
+++ b/docs/NUMEROS DE ASIGNACION DE EXPEDIENTES TEDEFE.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wamp\www\federacion\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SIGLAS ASIGNADAS" sheetId="1" r:id="rId1"/>
@@ -1067,8 +1072,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1820,6 +1825,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1835,67 +1849,66 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1937,7 +1950,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1969,9 +1982,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2003,6 +2017,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2178,14 +2193,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
@@ -2194,14 +2209,14 @@
     <col min="6" max="6" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B2" s="36" t="s">
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="2:6">
+      <c r="C2" s="42"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2215,7 +2230,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2229,7 +2244,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>341</v>
       </c>
@@ -2243,7 +2258,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1">
+    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
@@ -2257,7 +2272,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1">
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="5" t="s">
         <v>110</v>
       </c>
@@ -2265,11 +2280,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="38" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="43" t="s">
         <v>348</v>
       </c>
-      <c r="C8" s="39"/>
+      <c r="C8" s="44"/>
       <c r="E8" s="5" t="s">
         <v>111</v>
       </c>
@@ -2277,7 +2292,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
@@ -2291,7 +2306,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -2305,7 +2320,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2319,7 +2334,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
@@ -2333,7 +2348,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
@@ -2347,7 +2362,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
@@ -2361,7 +2376,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
@@ -2375,7 +2390,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
@@ -2389,7 +2404,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -2403,7 +2418,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -2417,7 +2432,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>18</v>
       </c>
@@ -2431,7 +2446,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
@@ -2445,7 +2460,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
@@ -2459,7 +2474,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
@@ -2473,7 +2488,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
@@ -2487,7 +2502,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
@@ -2501,7 +2516,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15.75" thickBot="1">
+    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>24</v>
       </c>
@@ -2515,7 +2530,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="15.75" thickBot="1">
+    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>25</v>
       </c>
@@ -2523,19 +2538,19 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="39"/>
-    </row>
-    <row r="28" spans="2:6">
+      <c r="F27" s="44"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
@@ -2549,7 +2564,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
@@ -2563,7 +2578,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="15.75" thickBot="1">
+    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>29</v>
       </c>
@@ -2577,7 +2592,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>30</v>
       </c>
@@ -2587,7 +2602,7 @@
       <c r="E31" s="34"/>
       <c r="F31" s="35"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>31</v>
       </c>
@@ -2597,7 +2612,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
@@ -2605,7 +2620,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
@@ -2613,7 +2628,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>34</v>
       </c>
@@ -2621,7 +2636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>35</v>
       </c>
@@ -2629,7 +2644,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>36</v>
       </c>
@@ -2637,7 +2652,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>37</v>
       </c>
@@ -2645,7 +2660,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>38</v>
       </c>
@@ -2653,7 +2668,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>39</v>
       </c>
@@ -2661,7 +2676,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>40</v>
       </c>
@@ -2669,7 +2684,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>41</v>
       </c>
@@ -2677,7 +2692,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>42</v>
       </c>
@@ -2685,7 +2700,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="2:3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>43</v>
       </c>
@@ -2693,7 +2708,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="2:3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>44</v>
       </c>
@@ -2701,7 +2716,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>45</v>
       </c>
@@ -2709,7 +2724,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="2:3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>46</v>
       </c>
@@ -2717,7 +2732,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="2:3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>47</v>
       </c>
@@ -2725,7 +2740,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>48</v>
       </c>
@@ -2733,7 +2748,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>49</v>
       </c>
@@ -2741,7 +2756,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>50</v>
       </c>
@@ -2749,7 +2764,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="2:3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>51</v>
       </c>
@@ -2757,43 +2772,43 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="15.75">
-      <c r="B53" s="44" t="s">
+    <row r="53" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B53" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="36" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="15.75">
-      <c r="B54" s="44" t="s">
+    <row r="54" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B54" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="C54" s="42" t="s">
+      <c r="C54" s="37" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="2:3" ht="15.75">
-      <c r="B55" s="44" t="s">
+    <row r="55" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B55" s="39" t="s">
         <v>345</v>
       </c>
-      <c r="C55" s="42" t="s">
+      <c r="C55" s="37" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="15.75">
-      <c r="B56" s="44" t="s">
+    <row r="56" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B56" s="39" t="s">
         <v>346</v>
       </c>
-      <c r="C56" s="42" t="s">
+      <c r="C56" s="37" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="16.5" thickBot="1">
-      <c r="B57" s="45" t="s">
+    <row r="57" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="40" t="s">
         <v>347</v>
       </c>
-      <c r="C57" s="43" t="s">
+      <c r="C57" s="38" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2811,14 +2826,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
@@ -2826,21 +2841,21 @@
     <col min="4" max="6" width="40.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="3.75" hidden="1" customHeight="1">
+    <row r="1" spans="2:6" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="10"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="2:6" ht="35.25" hidden="1" customHeight="1">
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-    </row>
-    <row r="3" spans="2:6" s="1" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
+    <row r="2" spans="2:6" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+    </row>
+    <row r="3" spans="2:6" s="1" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="22"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25" t="s">
@@ -2849,7 +2864,7 @@
       <c r="E3" s="24"/>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="2:6" ht="22.5" customHeight="1">
+    <row r="4" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>92</v>
       </c>
@@ -2866,7 +2881,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="1" customFormat="1" ht="19.5" customHeight="1">
+    <row r="5" spans="2:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
         <v>4</v>
       </c>
@@ -2875,7 +2890,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="26"/>
     </row>
-    <row r="6" spans="2:6" ht="24" customHeight="1">
+    <row r="6" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>52</v>
       </c>
@@ -2892,7 +2907,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="24" customHeight="1">
+    <row r="7" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>53</v>
       </c>
@@ -2909,7 +2924,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="24" customHeight="1">
+    <row r="8" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>54</v>
       </c>
@@ -2926,7 +2941,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="24" customHeight="1">
+    <row r="9" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>72</v>
       </c>
@@ -2943,7 +2958,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="24" customHeight="1">
+    <row r="10" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>55</v>
       </c>
@@ -2960,7 +2975,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="24" customHeight="1">
+    <row r="11" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>56</v>
       </c>
@@ -2977,7 +2992,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="24" customHeight="1">
+    <row r="12" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>93</v>
       </c>
@@ -2994,7 +3009,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="24" customHeight="1">
+    <row r="13" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
         <v>57</v>
       </c>
@@ -3011,7 +3026,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="24" customHeight="1">
+    <row r="14" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
         <v>58</v>
       </c>
@@ -3028,7 +3043,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="24" customHeight="1">
+    <row r="15" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
         <v>59</v>
       </c>
@@ -3045,7 +3060,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="24" customHeight="1">
+    <row r="16" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>60</v>
       </c>
@@ -3062,7 +3077,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="24" customHeight="1">
+    <row r="17" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
         <v>61</v>
       </c>
@@ -3079,7 +3094,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="24" customHeight="1">
+    <row r="18" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
         <v>73</v>
       </c>
@@ -3096,7 +3111,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="24" customHeight="1">
+    <row r="19" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>62</v>
       </c>
@@ -3113,7 +3128,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="24" customHeight="1">
+    <row r="20" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
         <v>63</v>
       </c>
@@ -3130,7 +3145,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="24" customHeight="1">
+    <row r="21" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>64</v>
       </c>
@@ -3147,7 +3162,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="32.25" customHeight="1">
+    <row r="22" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="19" t="s">
         <v>65</v>
       </c>
@@ -3164,7 +3179,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="33" customHeight="1">
+    <row r="23" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
         <v>66</v>
       </c>
@@ -3181,7 +3196,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="24" customHeight="1">
+    <row r="24" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
         <v>67</v>
       </c>
@@ -3198,7 +3213,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="24" customHeight="1">
+    <row r="25" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
         <v>68</v>
       </c>
@@ -3215,7 +3230,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="24" customHeight="1">
+    <row r="26" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
         <v>69</v>
       </c>
@@ -3232,7 +3247,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="23.25" customHeight="1">
+    <row r="27" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="19" t="s">
         <v>70</v>
       </c>
@@ -3249,7 +3264,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="25.5" customHeight="1">
+    <row r="28" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="18" t="s">
         <v>71</v>
       </c>
@@ -3266,7 +3281,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="24.75" customHeight="1">
+    <row r="29" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="18" t="s">
         <v>74</v>
       </c>
@@ -3283,7 +3298,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="24" customHeight="1">
+    <row r="30" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="18" t="s">
         <v>75</v>
       </c>
@@ -3300,7 +3315,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="24.75" customHeight="1">
+    <row r="31" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="18" t="s">
         <v>76</v>
       </c>
@@ -3317,7 +3332,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="24" customHeight="1">
+    <row r="32" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
         <v>34</v>
       </c>
@@ -3334,7 +3349,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="31.5" customHeight="1">
+    <row r="33" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="19" t="s">
         <v>77</v>
       </c>
@@ -3351,7 +3366,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="24" customHeight="1" thickBot="1">
+    <row r="34" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="20" t="s">
         <v>78</v>
       </c>
@@ -3368,14 +3383,14 @@
         <v>225</v>
       </c>
     </row>
-    <row r="35" spans="2:6" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1">
+    <row r="35" spans="2:6" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="28"/>
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
       <c r="F35" s="29"/>
     </row>
-    <row r="36" spans="2:6" ht="27" customHeight="1">
+    <row r="36" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="30" t="s">
         <v>5</v>
       </c>
@@ -3384,7 +3399,7 @@
       <c r="E36" s="31"/>
       <c r="F36" s="32"/>
     </row>
-    <row r="37" spans="2:6" ht="24" customHeight="1">
+    <row r="37" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="18" t="s">
         <v>79</v>
       </c>
@@ -3401,7 +3416,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="24" customHeight="1">
+    <row r="38" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="18" t="s">
         <v>80</v>
       </c>
@@ -3418,7 +3433,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="24" customHeight="1">
+    <row r="39" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="18" t="s">
         <v>39</v>
       </c>
@@ -3435,7 +3450,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="24" customHeight="1">
+    <row r="40" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
         <v>81</v>
       </c>
@@ -3452,7 +3467,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="24" customHeight="1">
+    <row r="41" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="18" t="s">
         <v>82</v>
       </c>
@@ -3469,7 +3484,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="24" customHeight="1">
+    <row r="42" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="19" t="s">
         <v>83</v>
       </c>
@@ -3486,7 +3501,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="24" customHeight="1">
+    <row r="43" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="18" t="s">
         <v>84</v>
       </c>
@@ -3503,7 +3518,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="24" customHeight="1">
+    <row r="44" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="18" t="s">
         <v>44</v>
       </c>
@@ -3520,7 +3535,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="24" customHeight="1">
+    <row r="45" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="18" t="s">
         <v>85</v>
       </c>
@@ -3537,7 +3552,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="24" customHeight="1">
+    <row r="46" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="18" t="s">
         <v>86</v>
       </c>
@@ -3554,7 +3569,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="24" customHeight="1">
+    <row r="47" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="18" t="s">
         <v>87</v>
       </c>
@@ -3571,7 +3586,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="24" customHeight="1">
+    <row r="48" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="18" t="s">
         <v>48</v>
       </c>
@@ -3588,7 +3603,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="24" customHeight="1">
+    <row r="49" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="18" t="s">
         <v>88</v>
       </c>
@@ -3605,7 +3620,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="29.25" customHeight="1">
+    <row r="50" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="19" t="s">
         <v>89</v>
       </c>
@@ -3622,7 +3637,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="24" customHeight="1" thickBot="1">
+    <row r="51" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="20" t="s">
         <v>90</v>
       </c>
@@ -3639,14 +3654,14 @@
         <v>244</v>
       </c>
     </row>
-    <row r="52" spans="2:6" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1">
+    <row r="52" spans="2:6" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="28"/>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
       <c r="F52" s="29"/>
     </row>
-    <row r="53" spans="2:6" s="1" customFormat="1" ht="27.75" customHeight="1">
+    <row r="53" spans="2:6" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="30" t="s">
         <v>100</v>
       </c>
@@ -3655,7 +3670,7 @@
       <c r="E53" s="31"/>
       <c r="F53" s="32"/>
     </row>
-    <row r="54" spans="2:6" ht="24" customHeight="1">
+    <row r="54" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="18" t="s">
         <v>103</v>
       </c>
@@ -3668,7 +3683,7 @@
       </c>
       <c r="F54" s="26"/>
     </row>
-    <row r="55" spans="2:6" ht="24" customHeight="1">
+    <row r="55" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="18" t="s">
         <v>101</v>
       </c>
@@ -3681,7 +3696,7 @@
       </c>
       <c r="F55" s="26"/>
     </row>
-    <row r="56" spans="2:6" ht="24" customHeight="1">
+    <row r="56" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="18" t="s">
         <v>102</v>
       </c>
@@ -3694,7 +3709,7 @@
       </c>
       <c r="F56" s="26"/>
     </row>
-    <row r="57" spans="2:6" ht="24" customHeight="1">
+    <row r="57" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="18" t="s">
         <v>151</v>
       </c>
@@ -3707,7 +3722,7 @@
       </c>
       <c r="F57" s="26"/>
     </row>
-    <row r="58" spans="2:6" ht="24" customHeight="1" thickBot="1">
+    <row r="58" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B58" s="20" t="s">
         <v>152</v>
       </c>
@@ -3720,14 +3735,14 @@
       </c>
       <c r="F58" s="27"/>
     </row>
-    <row r="59" spans="2:6" ht="16.5">
+    <row r="59" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B59" s="11"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
     </row>
-    <row r="60" spans="2:6" ht="16.5">
+    <row r="60" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B60" s="11"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>

</xml_diff>